<commit_message>
agregue al excel los tiempos de los metodos mios y de july
</commit_message>
<xml_diff>
--- a/Codigo - Ejercicios de clase/TP2-ComplejidadComputacional/Metricas.xlsx
+++ b/Codigo - Ejercicios de clase/TP2-ComplejidadComputacional/Metricas.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\Workspace\Progra Avanzada\Codigo - Ejercicios de clase\TP2-ComplejidadComputacional\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="3915" xr2:uid="{ECDA49D9-3B32-472C-B882-ADEB2F6722A3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="3915"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Binomio de Newton</t>
   </si>
@@ -99,13 +94,70 @@
   </si>
   <si>
     <t>O(N*LOG(N))</t>
+  </si>
+  <si>
+    <t>Polinomio</t>
+  </si>
+  <si>
+    <t>Polinomio de pruebas: 123.0x^42 + 31.0x^41 + 23.0x^40 + 9.0x^39 + 5.0x^38 + 666.0x^37 + 89.0x^36 + 6.0x^35 + 5.0x^34 + 54.0x^33 + 89.0x^32 + 6.0x^31 + 5.0x^30 + 54.0x^29 + 89.0x^28 + 6.0x^27 + 5.0x^26 + 54.0x^25 + 89.0x^24 + 6.0x^23 + 5.0x^22 + 123.0x^21 + 31.0x^20 + 23.0x^19 + 9.0x^18 + 5.0x^17 + 666.0x^16 + 89.0x^15 + 6.0x^14 + 5.0x^13 + 54.0x^12 + 89.0x^11 + 6.0x^10 + 5.0x^9 + 54.0x^8 + 89.0x^7 + 6.0x^6 + 5.0x^5 + 54.0x^4 + 89.0x^3 + 6.0x^2 + 5.0x^1 + 54.0</t>
+  </si>
+  <si>
+    <t>X para pruebas: 45</t>
+  </si>
+  <si>
+    <t>evaluarMSucesivas</t>
+  </si>
+  <si>
+    <t>evaluarRecursiva</t>
+  </si>
+  <si>
+    <t>evaluarRecursivaPar</t>
+  </si>
+  <si>
+    <t>evaluarProgDinamica</t>
+  </si>
+  <si>
+    <t>evaluarMejorada</t>
+  </si>
+  <si>
+    <t>evaluarPow</t>
+  </si>
+  <si>
+    <t>evaluarHorner</t>
+  </si>
+  <si>
+    <t>20995 nanosegundos</t>
+  </si>
+  <si>
+    <t>113431 nanosegundos</t>
+  </si>
+  <si>
+    <t>36449 nanosegundos</t>
+  </si>
+  <si>
+    <t>4374 nanosegundos</t>
+  </si>
+  <si>
+    <t>2916 nanosegundos</t>
+  </si>
+  <si>
+    <t>9915 nanosegundos</t>
+  </si>
+  <si>
+    <t>1750 nanosegundos</t>
+  </si>
+  <si>
+    <t>O(N^4)</t>
+  </si>
+  <si>
+    <t>O(N^2/3)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,8 +194,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +221,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -307,26 +372,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -342,6 +394,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,7 +488,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -454,7 +540,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -648,181 +734,390 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDA0A12-2C47-490D-9707-69972F2EE928}">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="36.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1"/>
+    <col min="5" max="5" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="1"/>
+    <col min="7" max="7" width="12.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+    </row>
+    <row r="22" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A22" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+    </row>
+    <row r="23" spans="1:3" s="26" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+    </row>
+    <row r="24" spans="1:3" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="10"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A24:C24"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>

</xml_diff>